<commit_message>
Make asin unique in B_creation; add File_creation to create multiple A and B
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/dev/gal_dev/capstone/movie_mood/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2A267E-7CA4-8E4D-9AE0-1A406A5D9034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8E757C-1F5C-8C48-A998-52DAEF7D5A5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16360" yWindow="3460" windowWidth="21940" windowHeight="16020" activeTab="2" xr2:uid="{A94EF82D-298B-6243-A7DB-178C01F81566}"/>
+    <workbookView xWindow="16360" yWindow="3460" windowWidth="21940" windowHeight="16020" xr2:uid="{A94EF82D-298B-6243-A7DB-178C01F81566}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="249">
   <si>
     <t>Reviews removed</t>
   </si>
@@ -762,6 +762,18 @@
   </si>
   <si>
     <t>If this was the film that made Godzilla famous, he should have been assassinated.Indeed this film will leave you thinking after you leave the theater: Why did I waste my time on this?</t>
+  </si>
+  <si>
+    <t>Per review</t>
+  </si>
+  <si>
+    <t>Remove from</t>
+  </si>
+  <si>
+    <t>Corpus</t>
+  </si>
+  <si>
+    <t>Sentences removed</t>
   </si>
 </sst>
 </file>
@@ -1161,24 +1173,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14251269-7956-BF44-A046-F99264A2EE10}">
-  <dimension ref="B1:H2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="4.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="4" width="13.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="4.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1186,37 +1201,68 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2">
         <v>30</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>2964</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>141036</v>
       </c>
-      <c r="F2" s="3">
-        <f>E2/(D2+E2)</f>
+      <c r="G2" s="3">
+        <f>F2/(E2+F2)</f>
         <v>0.97941666666666671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" s="3">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>33808</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1046</v>
+      </c>
+      <c r="F3" s="2">
+        <v>14400</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3/(E3+F3)</f>
+        <v>0.93228020199404371</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AB769C-CBCC-2048-8A28-542351CFB21D}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>

</xml_diff>